<commit_message>
Changed to mapping spreadsheet
</commit_message>
<xml_diff>
--- a/apps/bfd-model/bfd-model-rif/src/main/java/gov/cms/bfd/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/apps/bfd-model/bfd-model-rif/src/main/java/gov/cms/bfd/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbrune/workspaces/bfd/beneficiary-fhir-data.git/apps/bfd-model/bfd-model-rif/src/main/java/gov/cms/bfd/model/rif/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07270CA3-D38B-6041-AA6F-870D2613403E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E634C-17EF-CF4E-B332-A393FF417A45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14740" tabRatio="487" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14740" tabRatio="487" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -33790,7 +33790,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AML207"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
       <selection activeCell="F213" sqref="F213"/>
     </sheetView>
   </sheetViews>
@@ -52452,7 +52452,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AMK280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+    <sheetView topLeftCell="A262" workbookViewId="0">
       <selection activeCell="I269" sqref="I269"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added fake data to the resources for beneficiary and beneficiary history files
</commit_message>
<xml_diff>
--- a/apps/bfd-model/bfd-model-rif/src/main/java/gov/cms/bfd/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/apps/bfd-model/bfd-model-rif/src/main/java/gov/cms/bfd/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbrune/workspaces/bfd/beneficiary-fhir-data.git/apps/bfd-model/bfd-model-rif/src/main/java/gov/cms/bfd/model/rif/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00537D73-7A06-F84F-9E6C-C578F227C48D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDB1EE4-6639-4641-BB84-C5CEEAF9B579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14740" tabRatio="487" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14740" tabRatio="487" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14017" uniqueCount="2681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14029" uniqueCount="2681">
   <si>
     <t>adjustmentReason</t>
   </si>
@@ -8089,7 +8089,7 @@
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="44">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -8365,6 +8365,12 @@
       <sz val="12"/>
       <color rgb="FF6B0001"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="46">
@@ -8879,7 +8885,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9323,6 +9329,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -33790,8 +33803,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AML207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="F213" sqref="F213"/>
+    <sheetView topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="A205" sqref="A205:A206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
@@ -41149,8 +41162,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AML29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
@@ -41822,6 +41835,70 @@
       <c r="L21" s="16"/>
       <c r="N21" s="8"/>
       <c r="AML21" s="2"/>
+    </row>
+    <row r="22" spans="1:14 1026:1026">
+      <c r="A22" s="185" t="s">
+        <v>2637</v>
+      </c>
+      <c r="B22" s="185" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C22" s="185">
+        <v>8</v>
+      </c>
+      <c r="D22" s="185" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E22" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="187">
+        <v>33314</v>
+      </c>
+      <c r="G22" s="185" t="s">
+        <v>2637</v>
+      </c>
+      <c r="H22" s="185" t="s">
+        <v>2656</v>
+      </c>
+      <c r="I22" s="185" t="s">
+        <v>2618</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="16"/>
+    </row>
+    <row r="23" spans="1:14 1026:1026">
+      <c r="A23" s="185" t="s">
+        <v>2668</v>
+      </c>
+      <c r="B23" s="185" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C23" s="185">
+        <v>8</v>
+      </c>
+      <c r="D23" s="185" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E23" s="186" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="187">
+        <v>36967</v>
+      </c>
+      <c r="G23" s="185" t="s">
+        <v>2668</v>
+      </c>
+      <c r="H23" s="185" t="s">
+        <v>2657</v>
+      </c>
+      <c r="I23" s="185" t="s">
+        <v>2658</v>
+      </c>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="16"/>
     </row>
     <row r="29" spans="1:14 1026:1026" ht="16">
       <c r="D29" s="133"/>

</xml_diff>

<commit_message>
Added fi document control num and fi original control num
</commit_message>
<xml_diff>
--- a/apps/bfd-model/bfd-model-rif/src/main/java/gov/cms/bfd/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/apps/bfd-model/bfd-model-rif/src/main/java/gov/cms/bfd/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbrune/workspaces/bfd/beneficiary-fhir-data.git/apps/bfd-model/bfd-model-rif/src/main/java/gov/cms/bfd/model/rif/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8459564B-5F88-DA4B-809B-811AA586D31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF4CAE6-FAD0-7B4D-8C1F-5F03E591F636}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14740" tabRatio="487" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14740" tabRatio="487" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14041" uniqueCount="2684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14111" uniqueCount="2690">
   <si>
     <t>adjustmentReason</t>
   </si>
@@ -8088,6 +8088,24 @@
   </si>
   <si>
     <t>clmControlNumber</t>
+  </si>
+  <si>
+    <t>FI Document Claim Control Number </t>
+  </si>
+  <si>
+    <t>FI Original Claim Control Number </t>
+  </si>
+  <si>
+    <t>FI_DOC_CLM_CNTL_NUM</t>
+  </si>
+  <si>
+    <t>FI_ORIG_CLM_CNTL_NUM</t>
+  </si>
+  <si>
+    <t>fiOriginalClaimControlNumber</t>
+  </si>
+  <si>
+    <t>fiDocumentClaimControlNumber</t>
   </si>
 </sst>
 </file>
@@ -8098,7 +8116,7 @@
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="49">
+  <fonts count="51">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -8412,6 +8430,19 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -8929,7 +8960,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9397,6 +9428,11 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -9888,7 +9924,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AMK104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+    <sheetView topLeftCell="A81" workbookViewId="0">
       <selection activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
@@ -14710,16 +14746,17 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:AMK135"/>
+  <dimension ref="A1:AMK136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="7" width="8.5" style="71"/>
-    <col min="8" max="9" width="8.5" style="73"/>
+    <col min="8" max="8" width="8.5" style="73"/>
+    <col min="9" max="9" width="32.6640625" style="73" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.5" style="71"/>
     <col min="12" max="12" width="8.5" style="99"/>
     <col min="13" max="1025" width="8.5" style="71"/>
@@ -20189,50 +20226,80 @@
       <c r="L129" s="81"/>
     </row>
     <row r="130" spans="1:12">
-      <c r="A130" s="82"/>
-      <c r="B130" s="82"/>
-      <c r="C130" s="83"/>
-      <c r="D130" s="83"/>
-      <c r="E130" s="97"/>
+      <c r="A130" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B130" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C130" s="83">
+        <v>23</v>
+      </c>
+      <c r="D130" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E130" s="196" t="s">
+        <v>1806</v>
+      </c>
       <c r="F130" s="82"/>
-      <c r="G130" s="82"/>
-      <c r="H130" s="86"/>
-      <c r="I130" s="86"/>
+      <c r="G130" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="H130" s="195" t="s">
+        <v>2684</v>
+      </c>
+      <c r="I130" s="86" t="s">
+        <v>2689</v>
+      </c>
       <c r="J130" s="80"/>
       <c r="K130" s="80"/>
       <c r="L130" s="88"/>
     </row>
     <row r="131" spans="1:12">
-      <c r="A131" s="82"/>
-      <c r="B131" s="82"/>
-      <c r="C131" s="83"/>
-      <c r="D131" s="83"/>
-      <c r="E131" s="97"/>
+      <c r="A131" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B131" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C131" s="83">
+        <v>23</v>
+      </c>
+      <c r="D131" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E131" s="196" t="s">
+        <v>1806</v>
+      </c>
       <c r="F131" s="82"/>
-      <c r="G131" s="82"/>
-      <c r="H131" s="86"/>
-      <c r="I131" s="86"/>
+      <c r="G131" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="H131" s="195" t="s">
+        <v>2685</v>
+      </c>
+      <c r="I131" s="86" t="s">
+        <v>2688</v>
+      </c>
       <c r="J131" s="80"/>
       <c r="K131" s="80"/>
       <c r="L131" s="88"/>
     </row>
-    <row r="132" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A132" s="82"/>
+    <row r="132" spans="1:12">
+      <c r="A132" s="197"/>
       <c r="B132" s="82"/>
       <c r="C132" s="83"/>
       <c r="D132" s="83"/>
-      <c r="E132" s="97"/>
+      <c r="E132" s="196"/>
       <c r="F132" s="82"/>
-      <c r="G132" s="82"/>
-      <c r="H132" s="194" t="s">
-        <v>1225</v>
-      </c>
-      <c r="I132" s="194"/>
-      <c r="J132" s="194"/>
-      <c r="K132" s="194"/>
-      <c r="L132" s="93"/>
-    </row>
-    <row r="133" spans="1:12">
+      <c r="G132" s="197"/>
+      <c r="H132" s="195"/>
+      <c r="I132" s="86"/>
+      <c r="J132" s="80"/>
+      <c r="K132" s="80"/>
+      <c r="L132" s="88"/>
+    </row>
+    <row r="133" spans="1:12" ht="14.5" customHeight="1">
       <c r="A133" s="82"/>
       <c r="B133" s="82"/>
       <c r="C133" s="83"/>
@@ -20240,17 +20307,13 @@
       <c r="E133" s="97"/>
       <c r="F133" s="82"/>
       <c r="G133" s="82"/>
-      <c r="H133" s="86" t="s">
-        <v>418</v>
-      </c>
-      <c r="I133" s="86"/>
-      <c r="J133" s="87" t="s">
-        <v>1733</v>
-      </c>
-      <c r="K133" s="87" t="s">
-        <v>1591</v>
-      </c>
-      <c r="L133" s="81"/>
+      <c r="H133" s="194" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I133" s="194"/>
+      <c r="J133" s="194"/>
+      <c r="K133" s="194"/>
+      <c r="L133" s="93"/>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="82"/>
@@ -20261,14 +20324,14 @@
       <c r="F134" s="82"/>
       <c r="G134" s="82"/>
       <c r="H134" s="86" t="s">
-        <v>1592</v>
+        <v>418</v>
       </c>
       <c r="I134" s="86"/>
       <c r="J134" s="87" t="s">
         <v>1733</v>
       </c>
       <c r="K134" s="87" t="s">
-        <v>1868</v>
+        <v>1591</v>
       </c>
       <c r="L134" s="81"/>
     </row>
@@ -20281,20 +20344,40 @@
       <c r="F135" s="82"/>
       <c r="G135" s="82"/>
       <c r="H135" s="86" t="s">
-        <v>1229</v>
+        <v>1592</v>
       </c>
       <c r="I135" s="86"/>
       <c r="J135" s="87" t="s">
+        <v>1733</v>
+      </c>
+      <c r="K135" s="87" t="s">
+        <v>1868</v>
+      </c>
+      <c r="L135" s="81"/>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136" s="82"/>
+      <c r="B136" s="82"/>
+      <c r="C136" s="83"/>
+      <c r="D136" s="83"/>
+      <c r="E136" s="97"/>
+      <c r="F136" s="82"/>
+      <c r="G136" s="82"/>
+      <c r="H136" s="86" t="s">
+        <v>1229</v>
+      </c>
+      <c r="I136" s="86"/>
+      <c r="J136" s="87" t="s">
         <v>1743</v>
       </c>
-      <c r="K135" s="87" t="s">
+      <c r="K136" s="87" t="s">
         <v>1632</v>
       </c>
-      <c r="L135" s="81"/>
+      <c r="L136" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H132:K132"/>
+    <mergeCell ref="H133:K133"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
@@ -20652,12 +20735,12 @@
     <hyperlink ref="G129" r:id="rId352" xr:uid="{00000000-0004-0000-0A00-00005F010000}"/>
     <hyperlink ref="J129" r:id="rId353" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0A00-000060010000}"/>
     <hyperlink ref="K129" r:id="rId354" location="ExplanationOfBenefit.item.careTeam.provider" xr:uid="{00000000-0004-0000-0A00-000061010000}"/>
-    <hyperlink ref="J133" r:id="rId355" xr:uid="{00000000-0004-0000-0A00-000062010000}"/>
-    <hyperlink ref="K133" r:id="rId356" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0A00-000063010000}"/>
-    <hyperlink ref="J134" r:id="rId357" xr:uid="{00000000-0004-0000-0A00-000064010000}"/>
-    <hyperlink ref="K134" r:id="rId358" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0A00-000065010000}"/>
-    <hyperlink ref="J135" r:id="rId359" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0A00-000066010000}"/>
-    <hyperlink ref="K135" r:id="rId360" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0A00-000067010000}"/>
+    <hyperlink ref="J134" r:id="rId355" xr:uid="{00000000-0004-0000-0A00-000062010000}"/>
+    <hyperlink ref="K134" r:id="rId356" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0A00-000063010000}"/>
+    <hyperlink ref="J135" r:id="rId357" xr:uid="{00000000-0004-0000-0A00-000064010000}"/>
+    <hyperlink ref="K135" r:id="rId358" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0A00-000065010000}"/>
+    <hyperlink ref="J136" r:id="rId359" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0A00-000066010000}"/>
+    <hyperlink ref="K136" r:id="rId360" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0A00-000067010000}"/>
     <hyperlink ref="G7" r:id="rId361" xr:uid="{00000000-0004-0000-0A00-000068010000}"/>
     <hyperlink ref="J7" r:id="rId362" location="ExplanationOfBenefit" xr:uid="{00000000-0004-0000-0A00-000069010000}"/>
   </hyperlinks>
@@ -20673,10 +20756,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:AMK235"/>
+  <dimension ref="A1:AMK237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="A231" sqref="A231:I232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
@@ -29684,34 +29767,64 @@
       <c r="L230" s="81"/>
     </row>
     <row r="231" spans="1:12">
-      <c r="A231" s="82"/>
-      <c r="B231" s="82"/>
-      <c r="C231" s="83"/>
-      <c r="D231" s="83"/>
-      <c r="E231" s="92"/>
+      <c r="A231" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B231" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C231" s="83">
+        <v>23</v>
+      </c>
+      <c r="D231" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E231" s="196" t="s">
+        <v>1806</v>
+      </c>
       <c r="F231" s="82"/>
-      <c r="G231" s="82"/>
-      <c r="H231" s="86"/>
-      <c r="I231" s="86"/>
-      <c r="J231" s="80"/>
-      <c r="K231" s="80"/>
-      <c r="L231" s="88"/>
-    </row>
-    <row r="232" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A232" s="82"/>
-      <c r="B232" s="82"/>
-      <c r="C232" s="83"/>
-      <c r="D232" s="83"/>
-      <c r="E232" s="92"/>
+      <c r="G231" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="H231" s="195" t="s">
+        <v>2684</v>
+      </c>
+      <c r="I231" s="86" t="s">
+        <v>2689</v>
+      </c>
+      <c r="J231" s="87"/>
+      <c r="K231" s="87"/>
+      <c r="L231" s="81"/>
+    </row>
+    <row r="232" spans="1:12">
+      <c r="A232" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B232" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C232" s="83">
+        <v>23</v>
+      </c>
+      <c r="D232" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E232" s="196" t="s">
+        <v>1806</v>
+      </c>
       <c r="F232" s="82"/>
-      <c r="G232" s="82"/>
-      <c r="H232" s="194" t="s">
-        <v>1225</v>
-      </c>
-      <c r="I232" s="194"/>
-      <c r="J232" s="194"/>
-      <c r="K232" s="194"/>
-      <c r="L232" s="93"/>
+      <c r="G232" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="H232" s="195" t="s">
+        <v>2685</v>
+      </c>
+      <c r="I232" s="86" t="s">
+        <v>2688</v>
+      </c>
+      <c r="J232" s="87"/>
+      <c r="K232" s="87"/>
+      <c r="L232" s="81"/>
     </row>
     <row r="233" spans="1:12">
       <c r="A233" s="82"/>
@@ -29721,19 +29834,13 @@
       <c r="E233" s="92"/>
       <c r="F233" s="82"/>
       <c r="G233" s="82"/>
-      <c r="H233" s="86" t="s">
-        <v>418</v>
-      </c>
+      <c r="H233" s="86"/>
       <c r="I233" s="86"/>
-      <c r="J233" s="87" t="s">
-        <v>1733</v>
-      </c>
-      <c r="K233" s="87" t="s">
-        <v>1591</v>
-      </c>
-      <c r="L233" s="81"/>
-    </row>
-    <row r="234" spans="1:12">
+      <c r="J233" s="80"/>
+      <c r="K233" s="80"/>
+      <c r="L233" s="88"/>
+    </row>
+    <row r="234" spans="1:12" ht="14.5" customHeight="1">
       <c r="A234" s="82"/>
       <c r="B234" s="82"/>
       <c r="C234" s="83"/>
@@ -29741,17 +29848,13 @@
       <c r="E234" s="92"/>
       <c r="F234" s="82"/>
       <c r="G234" s="82"/>
-      <c r="H234" s="86" t="s">
-        <v>1592</v>
-      </c>
-      <c r="I234" s="86"/>
-      <c r="J234" s="87" t="s">
-        <v>1733</v>
-      </c>
-      <c r="K234" s="87" t="s">
-        <v>1868</v>
-      </c>
-      <c r="L234" s="81"/>
+      <c r="H234" s="194" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I234" s="194"/>
+      <c r="J234" s="194"/>
+      <c r="K234" s="194"/>
+      <c r="L234" s="93"/>
     </row>
     <row r="235" spans="1:12">
       <c r="A235" s="82"/>
@@ -29762,20 +29865,60 @@
       <c r="F235" s="82"/>
       <c r="G235" s="82"/>
       <c r="H235" s="86" t="s">
-        <v>1229</v>
+        <v>418</v>
       </c>
       <c r="I235" s="86"/>
       <c r="J235" s="87" t="s">
+        <v>1733</v>
+      </c>
+      <c r="K235" s="87" t="s">
+        <v>1591</v>
+      </c>
+      <c r="L235" s="81"/>
+    </row>
+    <row r="236" spans="1:12">
+      <c r="A236" s="82"/>
+      <c r="B236" s="82"/>
+      <c r="C236" s="83"/>
+      <c r="D236" s="83"/>
+      <c r="E236" s="92"/>
+      <c r="F236" s="82"/>
+      <c r="G236" s="82"/>
+      <c r="H236" s="86" t="s">
+        <v>1592</v>
+      </c>
+      <c r="I236" s="86"/>
+      <c r="J236" s="87" t="s">
+        <v>1733</v>
+      </c>
+      <c r="K236" s="87" t="s">
+        <v>1868</v>
+      </c>
+      <c r="L236" s="81"/>
+    </row>
+    <row r="237" spans="1:12">
+      <c r="A237" s="82"/>
+      <c r="B237" s="82"/>
+      <c r="C237" s="83"/>
+      <c r="D237" s="83"/>
+      <c r="E237" s="92"/>
+      <c r="F237" s="82"/>
+      <c r="G237" s="82"/>
+      <c r="H237" s="86" t="s">
+        <v>1229</v>
+      </c>
+      <c r="I237" s="86"/>
+      <c r="J237" s="87" t="s">
         <v>1743</v>
       </c>
-      <c r="K235" s="87" t="s">
+      <c r="K237" s="87" t="s">
         <v>1632</v>
       </c>
-      <c r="L235" s="81"/>
+      <c r="L237" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H232:K232"/>
+    <mergeCell ref="H234:K234"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
@@ -30422,12 +30565,12 @@
     <hyperlink ref="G230" r:id="rId641" xr:uid="{00000000-0004-0000-0B00-000080020000}"/>
     <hyperlink ref="J230" r:id="rId642" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0B00-000081020000}"/>
     <hyperlink ref="K230" r:id="rId643" location="ExplanationOfBenefit.item.careTeam.provider" xr:uid="{00000000-0004-0000-0B00-000082020000}"/>
-    <hyperlink ref="J233" r:id="rId644" xr:uid="{00000000-0004-0000-0B00-000083020000}"/>
-    <hyperlink ref="K233" r:id="rId645" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0B00-000084020000}"/>
-    <hyperlink ref="J234" r:id="rId646" xr:uid="{00000000-0004-0000-0B00-000085020000}"/>
-    <hyperlink ref="K234" r:id="rId647" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0B00-000086020000}"/>
-    <hyperlink ref="J235" r:id="rId648" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0B00-000087020000}"/>
-    <hyperlink ref="K235" r:id="rId649" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0B00-000088020000}"/>
+    <hyperlink ref="J235" r:id="rId644" xr:uid="{00000000-0004-0000-0B00-000083020000}"/>
+    <hyperlink ref="K235" r:id="rId645" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0B00-000084020000}"/>
+    <hyperlink ref="J236" r:id="rId646" xr:uid="{00000000-0004-0000-0B00-000085020000}"/>
+    <hyperlink ref="K236" r:id="rId647" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0B00-000086020000}"/>
+    <hyperlink ref="J237" r:id="rId648" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0B00-000087020000}"/>
+    <hyperlink ref="K237" r:id="rId649" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0B00-000088020000}"/>
     <hyperlink ref="G7" r:id="rId650" xr:uid="{00000000-0004-0000-0B00-000089020000}"/>
     <hyperlink ref="J7" r:id="rId651" location="ExplanationOfBenefit" xr:uid="{00000000-0004-0000-0B00-00008A020000}"/>
   </hyperlinks>
@@ -52648,10 +52791,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:AMK280"/>
+  <dimension ref="A1:AMK282"/>
   <sheetViews>
     <sheetView topLeftCell="A262" workbookViewId="0">
-      <selection activeCell="I269" sqref="I269"/>
+      <selection activeCell="A276" sqref="A276:I277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
@@ -62197,88 +62340,148 @@
       <c r="L275" s="16"/>
     </row>
     <row r="276" spans="1:12">
-      <c r="A276" s="14"/>
-      <c r="B276" s="14"/>
-      <c r="C276" s="17"/>
-      <c r="D276" s="17"/>
-      <c r="E276" s="23"/>
-      <c r="F276" s="14"/>
-      <c r="G276" s="14"/>
-      <c r="H276" s="27"/>
-      <c r="I276" s="27"/>
+      <c r="A276" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B276" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C276" s="83">
+        <v>23</v>
+      </c>
+      <c r="D276" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E276" s="196" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F276" s="82"/>
+      <c r="G276" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="H276" s="195" t="s">
+        <v>2684</v>
+      </c>
+      <c r="I276" s="86" t="s">
+        <v>2689</v>
+      </c>
       <c r="J276" s="15"/>
       <c r="K276" s="15"/>
       <c r="L276" s="16"/>
     </row>
-    <row r="277" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A277" s="64"/>
-      <c r="B277" s="64"/>
-      <c r="C277" s="65"/>
-      <c r="D277" s="65"/>
-      <c r="E277" s="66"/>
-      <c r="F277" s="14"/>
-      <c r="G277" s="14"/>
-      <c r="H277" s="192" t="s">
-        <v>1225</v>
-      </c>
-      <c r="I277" s="192"/>
-      <c r="J277" s="192"/>
-      <c r="K277" s="192"/>
-      <c r="L277" s="34"/>
+    <row r="277" spans="1:12">
+      <c r="A277" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B277" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C277" s="83">
+        <v>23</v>
+      </c>
+      <c r="D277" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E277" s="196" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F277" s="82"/>
+      <c r="G277" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="H277" s="195" t="s">
+        <v>2685</v>
+      </c>
+      <c r="I277" s="86" t="s">
+        <v>2688</v>
+      </c>
+      <c r="J277" s="15"/>
+      <c r="K277" s="15"/>
+      <c r="L277" s="16"/>
     </row>
     <row r="278" spans="1:12">
-      <c r="A278" s="67"/>
-      <c r="B278" s="67"/>
-      <c r="C278" s="68"/>
-      <c r="D278" s="68"/>
-      <c r="E278" s="69"/>
+      <c r="A278" s="14"/>
+      <c r="B278" s="14"/>
+      <c r="C278" s="17"/>
+      <c r="D278" s="17"/>
+      <c r="E278" s="23"/>
       <c r="F278" s="14"/>
       <c r="G278" s="14"/>
-      <c r="H278" s="27" t="s">
-        <v>418</v>
-      </c>
+      <c r="H278" s="27"/>
       <c r="I278" s="27"/>
-      <c r="J278" s="21" t="s">
-        <v>1733</v>
-      </c>
-      <c r="K278" s="21" t="s">
-        <v>1591</v>
-      </c>
+      <c r="J278" s="15"/>
+      <c r="K278" s="15"/>
       <c r="L278" s="16"/>
     </row>
-    <row r="279" spans="1:12">
+    <row r="279" spans="1:12" ht="14.5" customHeight="1">
+      <c r="A279" s="64"/>
+      <c r="B279" s="64"/>
+      <c r="C279" s="65"/>
+      <c r="D279" s="65"/>
+      <c r="E279" s="66"/>
       <c r="F279" s="14"/>
       <c r="G279" s="14"/>
-      <c r="H279" s="27" t="s">
-        <v>1592</v>
-      </c>
-      <c r="I279" s="27"/>
-      <c r="J279" s="21" t="s">
-        <v>1733</v>
-      </c>
-      <c r="K279" s="21" t="s">
-        <v>1868</v>
-      </c>
-      <c r="L279" s="16"/>
+      <c r="H279" s="192" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I279" s="192"/>
+      <c r="J279" s="192"/>
+      <c r="K279" s="192"/>
+      <c r="L279" s="34"/>
     </row>
     <row r="280" spans="1:12">
+      <c r="A280" s="67"/>
+      <c r="B280" s="67"/>
+      <c r="C280" s="68"/>
+      <c r="D280" s="68"/>
+      <c r="E280" s="69"/>
       <c r="F280" s="14"/>
       <c r="G280" s="14"/>
       <c r="H280" s="27" t="s">
-        <v>1229</v>
+        <v>418</v>
       </c>
       <c r="I280" s="27"/>
       <c r="J280" s="21" t="s">
+        <v>1733</v>
+      </c>
+      <c r="K280" s="21" t="s">
+        <v>1591</v>
+      </c>
+      <c r="L280" s="16"/>
+    </row>
+    <row r="281" spans="1:12">
+      <c r="F281" s="14"/>
+      <c r="G281" s="14"/>
+      <c r="H281" s="27" t="s">
+        <v>1592</v>
+      </c>
+      <c r="I281" s="27"/>
+      <c r="J281" s="21" t="s">
+        <v>1733</v>
+      </c>
+      <c r="K281" s="21" t="s">
+        <v>1868</v>
+      </c>
+      <c r="L281" s="16"/>
+    </row>
+    <row r="282" spans="1:12">
+      <c r="F282" s="14"/>
+      <c r="G282" s="14"/>
+      <c r="H282" s="27" t="s">
+        <v>1229</v>
+      </c>
+      <c r="I282" s="27"/>
+      <c r="J282" s="21" t="s">
         <v>1743</v>
       </c>
-      <c r="K280" s="21" t="s">
+      <c r="K282" s="21" t="s">
         <v>1632</v>
       </c>
-      <c r="L280" s="16"/>
+      <c r="L282" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H277:K277"/>
+    <mergeCell ref="H279:K279"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
@@ -63044,12 +63247,12 @@
     <hyperlink ref="G274" r:id="rId760" xr:uid="{00000000-0004-0000-0600-0000F7020000}"/>
     <hyperlink ref="J274" r:id="rId761" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0600-0000F8020000}"/>
     <hyperlink ref="K274" r:id="rId762" location="ExplanationOfBenefit.item.careTeam.provider" xr:uid="{00000000-0004-0000-0600-0000F9020000}"/>
-    <hyperlink ref="J278" r:id="rId763" xr:uid="{00000000-0004-0000-0600-0000FA020000}"/>
-    <hyperlink ref="K278" r:id="rId764" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0600-0000FB020000}"/>
-    <hyperlink ref="J279" r:id="rId765" xr:uid="{00000000-0004-0000-0600-0000FC020000}"/>
-    <hyperlink ref="K279" r:id="rId766" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0600-0000FD020000}"/>
-    <hyperlink ref="J280" r:id="rId767" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0600-0000FE020000}"/>
-    <hyperlink ref="K280" r:id="rId768" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0600-0000FF020000}"/>
+    <hyperlink ref="J280" r:id="rId763" xr:uid="{00000000-0004-0000-0600-0000FA020000}"/>
+    <hyperlink ref="K280" r:id="rId764" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0600-0000FB020000}"/>
+    <hyperlink ref="J281" r:id="rId765" xr:uid="{00000000-0004-0000-0600-0000FC020000}"/>
+    <hyperlink ref="K281" r:id="rId766" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0600-0000FD020000}"/>
+    <hyperlink ref="J282" r:id="rId767" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0600-0000FE020000}"/>
+    <hyperlink ref="K282" r:id="rId768" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0600-0000FF020000}"/>
     <hyperlink ref="G7" r:id="rId769" xr:uid="{00000000-0004-0000-0600-000000030000}"/>
     <hyperlink ref="J7" r:id="rId770" location="ExplanationOfBenefit" xr:uid="{00000000-0004-0000-0600-000001030000}"/>
   </hyperlinks>
@@ -63065,10 +63268,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:AMK239"/>
+  <dimension ref="A1:AMK241"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="A235" sqref="A235:I236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
@@ -71167,34 +71370,64 @@
       <c r="L234" s="16"/>
     </row>
     <row r="235" spans="1:12">
-      <c r="A235" s="14"/>
-      <c r="B235" s="14"/>
-      <c r="C235" s="17"/>
-      <c r="D235" s="17"/>
-      <c r="E235" s="23"/>
-      <c r="F235" s="14"/>
-      <c r="G235" s="14"/>
-      <c r="H235" s="27"/>
-      <c r="I235" s="27"/>
-      <c r="J235" s="15"/>
-      <c r="K235" s="15"/>
-      <c r="L235" s="29"/>
-    </row>
-    <row r="236" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A236" s="14"/>
-      <c r="B236" s="14"/>
-      <c r="C236" s="17"/>
-      <c r="D236" s="17"/>
-      <c r="E236" s="23"/>
-      <c r="F236" s="14"/>
-      <c r="G236" s="14"/>
-      <c r="H236" s="192" t="s">
-        <v>1225</v>
-      </c>
-      <c r="I236" s="192"/>
-      <c r="J236" s="192"/>
-      <c r="K236" s="192"/>
-      <c r="L236" s="34"/>
+      <c r="A235" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B235" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C235" s="83">
+        <v>23</v>
+      </c>
+      <c r="D235" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E235" s="196" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F235" s="82"/>
+      <c r="G235" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="H235" s="195" t="s">
+        <v>2684</v>
+      </c>
+      <c r="I235" s="86" t="s">
+        <v>2689</v>
+      </c>
+      <c r="J235" s="21"/>
+      <c r="K235" s="21"/>
+      <c r="L235" s="16"/>
+    </row>
+    <row r="236" spans="1:12">
+      <c r="A236" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B236" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C236" s="83">
+        <v>23</v>
+      </c>
+      <c r="D236" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E236" s="196" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F236" s="82"/>
+      <c r="G236" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="H236" s="195" t="s">
+        <v>2685</v>
+      </c>
+      <c r="I236" s="86" t="s">
+        <v>2688</v>
+      </c>
+      <c r="J236" s="21"/>
+      <c r="K236" s="21"/>
+      <c r="L236" s="16"/>
     </row>
     <row r="237" spans="1:12">
       <c r="A237" s="14"/>
@@ -71204,19 +71437,13 @@
       <c r="E237" s="23"/>
       <c r="F237" s="14"/>
       <c r="G237" s="14"/>
-      <c r="H237" s="27" t="s">
-        <v>1228</v>
-      </c>
+      <c r="H237" s="27"/>
       <c r="I237" s="27"/>
-      <c r="J237" s="21" t="s">
-        <v>1733</v>
-      </c>
-      <c r="K237" s="21" t="s">
-        <v>1591</v>
-      </c>
-      <c r="L237" s="16"/>
-    </row>
-    <row r="238" spans="1:12">
+      <c r="J237" s="15"/>
+      <c r="K237" s="15"/>
+      <c r="L237" s="29"/>
+    </row>
+    <row r="238" spans="1:12" ht="14.5" customHeight="1">
       <c r="A238" s="14"/>
       <c r="B238" s="14"/>
       <c r="C238" s="17"/>
@@ -71224,17 +71451,13 @@
       <c r="E238" s="23"/>
       <c r="F238" s="14"/>
       <c r="G238" s="14"/>
-      <c r="H238" s="27" t="s">
-        <v>1592</v>
-      </c>
-      <c r="I238" s="27"/>
-      <c r="J238" s="21" t="s">
-        <v>1733</v>
-      </c>
-      <c r="K238" s="21" t="s">
-        <v>1868</v>
-      </c>
-      <c r="L238" s="16"/>
+      <c r="H238" s="192" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I238" s="192"/>
+      <c r="J238" s="192"/>
+      <c r="K238" s="192"/>
+      <c r="L238" s="34"/>
     </row>
     <row r="239" spans="1:12">
       <c r="A239" s="14"/>
@@ -71245,20 +71468,60 @@
       <c r="F239" s="14"/>
       <c r="G239" s="14"/>
       <c r="H239" s="27" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="I239" s="27"/>
       <c r="J239" s="21" t="s">
+        <v>1733</v>
+      </c>
+      <c r="K239" s="21" t="s">
+        <v>1591</v>
+      </c>
+      <c r="L239" s="16"/>
+    </row>
+    <row r="240" spans="1:12">
+      <c r="A240" s="14"/>
+      <c r="B240" s="14"/>
+      <c r="C240" s="17"/>
+      <c r="D240" s="17"/>
+      <c r="E240" s="23"/>
+      <c r="F240" s="14"/>
+      <c r="G240" s="14"/>
+      <c r="H240" s="27" t="s">
+        <v>1592</v>
+      </c>
+      <c r="I240" s="27"/>
+      <c r="J240" s="21" t="s">
+        <v>1733</v>
+      </c>
+      <c r="K240" s="21" t="s">
+        <v>1868</v>
+      </c>
+      <c r="L240" s="16"/>
+    </row>
+    <row r="241" spans="1:12">
+      <c r="A241" s="14"/>
+      <c r="B241" s="14"/>
+      <c r="C241" s="17"/>
+      <c r="D241" s="17"/>
+      <c r="E241" s="23"/>
+      <c r="F241" s="14"/>
+      <c r="G241" s="14"/>
+      <c r="H241" s="27" t="s">
+        <v>1229</v>
+      </c>
+      <c r="I241" s="27"/>
+      <c r="J241" s="21" t="s">
         <v>1743</v>
       </c>
-      <c r="K239" s="21" t="s">
+      <c r="K241" s="21" t="s">
         <v>1632</v>
       </c>
-      <c r="L239" s="16"/>
+      <c r="L241" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H236:K236"/>
+    <mergeCell ref="H238:K238"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
@@ -71912,12 +72175,12 @@
     <hyperlink ref="G234" r:id="rId648" xr:uid="{00000000-0004-0000-0700-000087020000}"/>
     <hyperlink ref="J234" r:id="rId649" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0700-000088020000}"/>
     <hyperlink ref="K234" r:id="rId650" location="ExplanationOfBenefit.item.careTeam.provider" xr:uid="{00000000-0004-0000-0700-000089020000}"/>
-    <hyperlink ref="J237" r:id="rId651" xr:uid="{00000000-0004-0000-0700-00008A020000}"/>
-    <hyperlink ref="K237" r:id="rId652" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0700-00008B020000}"/>
-    <hyperlink ref="J238" r:id="rId653" xr:uid="{00000000-0004-0000-0700-00008C020000}"/>
-    <hyperlink ref="K238" r:id="rId654" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0700-00008D020000}"/>
-    <hyperlink ref="J239" r:id="rId655" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0700-00008E020000}"/>
-    <hyperlink ref="K239" r:id="rId656" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0700-00008F020000}"/>
+    <hyperlink ref="J239" r:id="rId651" xr:uid="{00000000-0004-0000-0700-00008A020000}"/>
+    <hyperlink ref="K239" r:id="rId652" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0700-00008B020000}"/>
+    <hyperlink ref="J240" r:id="rId653" xr:uid="{00000000-0004-0000-0700-00008C020000}"/>
+    <hyperlink ref="K240" r:id="rId654" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0700-00008D020000}"/>
+    <hyperlink ref="J241" r:id="rId655" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0700-00008E020000}"/>
+    <hyperlink ref="K241" r:id="rId656" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0700-00008F020000}"/>
     <hyperlink ref="G7" r:id="rId657" xr:uid="{00000000-0004-0000-0700-000090020000}"/>
     <hyperlink ref="J7" r:id="rId658" location="ExplanationOfBenefit" xr:uid="{00000000-0004-0000-0700-000091020000}"/>
   </hyperlinks>
@@ -71933,19 +72196,22 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:AMK136"/>
+  <dimension ref="A1:AMK138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="8.5" style="71" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="71" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="71" customWidth="1"/>
     <col min="3" max="4" width="8.5" style="71"/>
     <col min="5" max="5" width="8.5" style="72"/>
-    <col min="6" max="7" width="8.5" style="71"/>
-    <col min="8" max="9" width="8.5" style="73"/>
+    <col min="6" max="6" width="8.5" style="71"/>
+    <col min="7" max="7" width="22.83203125" style="71" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49" style="73" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" style="73" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.5" style="71"/>
     <col min="12" max="12" width="8.5" style="74"/>
     <col min="13" max="1025" width="8.5" style="71"/>
@@ -77477,34 +77743,64 @@
       <c r="L131" s="81"/>
     </row>
     <row r="132" spans="1:12">
-      <c r="A132" s="82"/>
-      <c r="B132" s="82"/>
-      <c r="C132" s="83"/>
-      <c r="D132" s="83"/>
-      <c r="E132" s="92"/>
+      <c r="A132" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B132" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C132" s="83">
+        <v>23</v>
+      </c>
+      <c r="D132" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E132" s="196" t="s">
+        <v>1806</v>
+      </c>
       <c r="F132" s="82"/>
-      <c r="G132" s="82"/>
-      <c r="H132" s="86"/>
-      <c r="I132" s="86"/>
+      <c r="G132" s="197" t="s">
+        <v>2686</v>
+      </c>
+      <c r="H132" s="195" t="s">
+        <v>2684</v>
+      </c>
+      <c r="I132" s="86" t="s">
+        <v>2689</v>
+      </c>
       <c r="J132" s="80"/>
       <c r="K132" s="80"/>
       <c r="L132" s="81"/>
     </row>
-    <row r="133" spans="1:12" ht="14.5" customHeight="1">
-      <c r="A133" s="82"/>
-      <c r="B133" s="82"/>
-      <c r="C133" s="83"/>
-      <c r="D133" s="83"/>
-      <c r="E133" s="92"/>
+    <row r="133" spans="1:12">
+      <c r="A133" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B133" s="82" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C133" s="83">
+        <v>23</v>
+      </c>
+      <c r="D133" s="83" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E133" s="196" t="s">
+        <v>1806</v>
+      </c>
       <c r="F133" s="82"/>
-      <c r="G133" s="82"/>
-      <c r="H133" s="194" t="s">
-        <v>1225</v>
-      </c>
-      <c r="I133" s="194"/>
-      <c r="J133" s="194"/>
-      <c r="K133" s="194"/>
-      <c r="L133" s="93"/>
+      <c r="G133" s="197" t="s">
+        <v>2687</v>
+      </c>
+      <c r="H133" s="195" t="s">
+        <v>2685</v>
+      </c>
+      <c r="I133" s="86" t="s">
+        <v>2688</v>
+      </c>
+      <c r="J133" s="80"/>
+      <c r="K133" s="80"/>
+      <c r="L133" s="81"/>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="82"/>
@@ -77514,19 +77810,13 @@
       <c r="E134" s="92"/>
       <c r="F134" s="82"/>
       <c r="G134" s="82"/>
-      <c r="H134" s="86" t="s">
-        <v>418</v>
-      </c>
+      <c r="H134" s="86"/>
       <c r="I134" s="86"/>
-      <c r="J134" s="87" t="s">
-        <v>1733</v>
-      </c>
-      <c r="K134" s="87" t="s">
-        <v>1591</v>
-      </c>
+      <c r="J134" s="80"/>
+      <c r="K134" s="80"/>
       <c r="L134" s="81"/>
     </row>
-    <row r="135" spans="1:12">
+    <row r="135" spans="1:12" ht="14.5" customHeight="1">
       <c r="A135" s="82"/>
       <c r="B135" s="82"/>
       <c r="C135" s="83"/>
@@ -77534,17 +77824,13 @@
       <c r="E135" s="92"/>
       <c r="F135" s="82"/>
       <c r="G135" s="82"/>
-      <c r="H135" s="86" t="s">
-        <v>1592</v>
-      </c>
-      <c r="I135" s="86"/>
-      <c r="J135" s="87" t="s">
-        <v>1733</v>
-      </c>
-      <c r="K135" s="87" t="s">
-        <v>1868</v>
-      </c>
-      <c r="L135" s="81"/>
+      <c r="H135" s="194" t="s">
+        <v>1225</v>
+      </c>
+      <c r="I135" s="194"/>
+      <c r="J135" s="194"/>
+      <c r="K135" s="194"/>
+      <c r="L135" s="93"/>
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="82"/>
@@ -77555,20 +77841,60 @@
       <c r="F136" s="82"/>
       <c r="G136" s="82"/>
       <c r="H136" s="86" t="s">
-        <v>1229</v>
+        <v>418</v>
       </c>
       <c r="I136" s="86"/>
       <c r="J136" s="87" t="s">
+        <v>1733</v>
+      </c>
+      <c r="K136" s="87" t="s">
+        <v>1591</v>
+      </c>
+      <c r="L136" s="81"/>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="A137" s="82"/>
+      <c r="B137" s="82"/>
+      <c r="C137" s="83"/>
+      <c r="D137" s="83"/>
+      <c r="E137" s="92"/>
+      <c r="F137" s="82"/>
+      <c r="G137" s="82"/>
+      <c r="H137" s="86" t="s">
+        <v>1592</v>
+      </c>
+      <c r="I137" s="86"/>
+      <c r="J137" s="87" t="s">
+        <v>1733</v>
+      </c>
+      <c r="K137" s="87" t="s">
+        <v>1868</v>
+      </c>
+      <c r="L137" s="81"/>
+    </row>
+    <row r="138" spans="1:12">
+      <c r="A138" s="82"/>
+      <c r="B138" s="82"/>
+      <c r="C138" s="83"/>
+      <c r="D138" s="83"/>
+      <c r="E138" s="92"/>
+      <c r="F138" s="82"/>
+      <c r="G138" s="82"/>
+      <c r="H138" s="86" t="s">
+        <v>1229</v>
+      </c>
+      <c r="I138" s="86"/>
+      <c r="J138" s="87" t="s">
         <v>1743</v>
       </c>
-      <c r="K136" s="87" t="s">
+      <c r="K138" s="87" t="s">
         <v>1632</v>
       </c>
-      <c r="L136" s="81"/>
+      <c r="L138" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H133:K133"/>
+    <mergeCell ref="H135:K135"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
@@ -77925,12 +78251,12 @@
     <hyperlink ref="G131" r:id="rId351" xr:uid="{00000000-0004-0000-0800-00005E010000}"/>
     <hyperlink ref="J131" r:id="rId352" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0800-00005F010000}"/>
     <hyperlink ref="K131" r:id="rId353" location="ExplanationOfBenefit.item.careTeam.provider" xr:uid="{00000000-0004-0000-0800-000060010000}"/>
-    <hyperlink ref="J134" r:id="rId354" xr:uid="{00000000-0004-0000-0800-000061010000}"/>
-    <hyperlink ref="K134" r:id="rId355" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0800-000062010000}"/>
-    <hyperlink ref="J135" r:id="rId356" xr:uid="{00000000-0004-0000-0800-000063010000}"/>
-    <hyperlink ref="K135" r:id="rId357" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0800-000064010000}"/>
-    <hyperlink ref="J136" r:id="rId358" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0800-000065010000}"/>
-    <hyperlink ref="K136" r:id="rId359" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0800-000066010000}"/>
+    <hyperlink ref="J136" r:id="rId354" xr:uid="{00000000-0004-0000-0800-000061010000}"/>
+    <hyperlink ref="K136" r:id="rId355" location="ExplanationOfBenefit.coverage.coverage" xr:uid="{00000000-0004-0000-0800-000062010000}"/>
+    <hyperlink ref="J137" r:id="rId356" xr:uid="{00000000-0004-0000-0800-000063010000}"/>
+    <hyperlink ref="K137" r:id="rId357" location="ExplanationOfBenefit.status" xr:uid="{00000000-0004-0000-0800-000064010000}"/>
+    <hyperlink ref="J138" r:id="rId358" location="ExplanationOfBenefit.item" xr:uid="{00000000-0004-0000-0800-000065010000}"/>
+    <hyperlink ref="K138" r:id="rId359" location="ExplanationOfBenefit.item.detail.type" xr:uid="{00000000-0004-0000-0800-000066010000}"/>
     <hyperlink ref="G7" r:id="rId360" xr:uid="{00000000-0004-0000-0800-000067010000}"/>
     <hyperlink ref="J7" r:id="rId361" location="ExplanationOfBenefit" xr:uid="{00000000-0004-0000-0800-000068010000}"/>
   </hyperlinks>

</xml_diff>